<commit_message>
base de datos con sedes actualizadas
</commit_message>
<xml_diff>
--- a/docs/STAFF ODONTOLOGICO RED COA FEBRERO 2020.xlsx
+++ b/docs/STAFF ODONTOLOGICO RED COA FEBRERO 2020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="STAFF CD RED COA" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,7 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'STAFF CD RED COA'!$A$12:$H$225</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Extract" vbProcedure="false">'staff cd red coa'!#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'STAFF CD RED COA'!$A$12:$H$225</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'STAFF CD RED COA'!$A$12:$H$225</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -3290,9 +3291,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>991440</xdr:colOff>
+      <xdr:colOff>991080</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>313560</xdr:rowOff>
+      <xdr:rowOff>313200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3306,7 +3307,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="67320" y="100800"/>
-          <a:ext cx="5410080" cy="1250640"/>
+          <a:ext cx="5438520" cy="1250280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3332,9 +3333,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2276280</xdr:colOff>
+      <xdr:colOff>2275920</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>64080</xdr:rowOff>
+      <xdr:rowOff>63720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3348,7 +3349,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="38160" y="57240"/>
-          <a:ext cx="2771280" cy="768600"/>
+          <a:ext cx="2770920" cy="768240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3371,22 +3372,22 @@
   </sheetPr>
   <dimension ref="A1:I226"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="0" ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="12" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A2:G214"/>
+      <selection pane="bottomLeft" activeCell="C167" activeCellId="0" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.9919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.3481781376518"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="3" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="72.3036437246964"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="72.9473684210526"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -8414,15 +8415,15 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H16" activeCellId="1" sqref="A2:G214 H16"/>
+      <selection pane="bottomLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="31" width="6"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9514170040486"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.3805668016194"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.7732793522267"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.3076923076923"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -8733,19 +8734,19 @@
   </sheetPr>
   <dimension ref="A1:G214"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G214" activeCellId="0" sqref="A2:G214"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G214" activeCellId="0" sqref="G214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8056680161943"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5425101214575"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.6963562753036"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8137651821862"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13689,17 +13690,17 @@
   <dimension ref="B1:H8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="A2:G214"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="27" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
base de datos con cede central
</commit_message>
<xml_diff>
--- a/docs/STAFF ODONTOLOGICO RED COA FEBRERO 2020.xlsx
+++ b/docs/STAFF ODONTOLOGICO RED COA FEBRERO 2020.xlsx
@@ -5,19 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="STAFF CD RED COA" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="RETIRAR DE WEB" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Hoja1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Hoja5" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'STAFF CD RED COA'!$A$12:$H$225</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Extract" vbProcedure="false">'staff cd red coa'!#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'STAFF CD RED COA'!$A$12:$H$225</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'STAFF CD RED COA'!$A$12:$H$225</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'STAFF CD RED COA'!$A$12:$H$225</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2484" uniqueCount="729">
   <si>
     <t xml:space="preserve">STAFF ODONTOLÓGICO RED COA</t>
   </si>
@@ -1900,6 +1902,330 @@
   </si>
   <si>
     <t xml:space="preserve">ELIZABETH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APELLIDOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE(S)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N° RNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALABA CASTAÑEDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WESLEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFARO SHIGUETO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOWARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANGELES SOTELO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILAGROS ELISA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARROYO RONCAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZULA WONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORONEL AMADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMPANA MEDINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRIBILLERO DE PINHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROSSANA MARLENE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOMINGUEZ ESTRADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARTIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERNANDEZ CASTILLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JULIO IVAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERNANDEZ TORRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAROLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLORES MENA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GABRIEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GYGLI REINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WALTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LANFRANCO LEON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFREDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLERENA PEREZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOURDES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANRIQUE CHAVEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAROLINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARQUEZ MENDOZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALEXIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORTIZ PALOMINO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLIVERA MADGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUIS ENRIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIAGGIO BRAVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAGGIO BENAVIDES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SALAZAR GARCIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JAVIER FRANCISCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCARAFONE ALVIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GERSON GIANCARLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAFUR JIMENEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIVES BARRETO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZUIKO FELIX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIRUGÍA BUCAL Y MAXILO FACIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIÑA CARDENAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALMEIDA RUIZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLAUDIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AYRES TORANZO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANDREA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARCHANI MARQUEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILUZKA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROJAS AMADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARITZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SANTOS SALAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELENA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SANTOS ESCALANTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLAVER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARCE SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUBERTO GONZALO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAUCCA MONTOYA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CINTHYA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VADILLO PALACIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRISEL YULIANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VELEZMORO PEÑA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELVIRA VANESSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODONTOPEDIATRÍA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAFUR TAFUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALY MICHEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SILVA ALBIZURI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIVERA ALIAGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALVARO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAYMUNDO CALERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAMIREZ MASIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NATHALY MILAGROS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REHABILITACIÓN ORAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAZ MAYURI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAJARES MUÑOZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLAUDIA MAGALI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTAZU ALDANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSCOL GALLARDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERNANDO JAVIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENESES LOPEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUILLEN ASTETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CELSO ANTONIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GALVEZ CUBAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GISELA ELIZABETH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLORES RICARDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GABRIEL PEDRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLORES MORENO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARTHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARDENAS MARINO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTHER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALDERON VALENCIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIELA ZUNILDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAMONDE SEGURA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEYLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARRIOLA GUILLEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARMAS GALVEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NELSON MURICIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMARO RIVERA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIA YESENIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALVITEZ CABALLERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAMELA</t>
   </si>
 </sst>
 </file>
@@ -2594,7 +2920,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="157">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3207,6 +3533,22 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -3291,9 +3633,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>991080</xdr:colOff>
+      <xdr:colOff>990720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>313200</xdr:rowOff>
+      <xdr:rowOff>312840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3307,7 +3649,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="67320" y="100800"/>
-          <a:ext cx="5438520" cy="1250280"/>
+          <a:ext cx="5476320" cy="1249920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3333,9 +3675,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2275920</xdr:colOff>
+      <xdr:colOff>2275560</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>63720</xdr:rowOff>
+      <xdr:rowOff>63360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3349,7 +3691,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="38160" y="57240"/>
-          <a:ext cx="2770920" cy="768240"/>
+          <a:ext cx="2770560" cy="767880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3372,22 +3714,22 @@
   </sheetPr>
   <dimension ref="A1:I226"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="12" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="12" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C167" activeCellId="0" sqref="C167"/>
+      <selection pane="bottomLeft" activeCell="C220" activeCellId="1" sqref="H2:H66 C220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.9919028340081"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.3117408906883"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="3" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="72.9473684210526"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="73.5910931174089"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -8415,15 +8757,15 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="H16" activeCellId="0" sqref="H2:H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="31" width="6"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.3805668016194"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.7044534412956"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.3076923076923"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8461538461538"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -8735,17 +9077,17 @@
   <dimension ref="A1:G214"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G214" activeCellId="0" sqref="G214"/>
+      <selection pane="topLeft" activeCell="G214" activeCellId="1" sqref="H2:H66 G214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.0283400809717"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -13690,17 +14032,17 @@
   <dimension ref="B1:H8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="1" sqref="H2:H66 E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="27" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -13847,4 +14189,1679 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H66"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="153" width="25.3603238866397"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="153" width="24.587044534413"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="153" width="30.6518218623482"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="153" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="153" width="36.085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="153" width="56.5587044534413"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="153" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="154" t="s">
+        <v>621</v>
+      </c>
+      <c r="B1" s="154" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1" s="154" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="154" t="s">
+        <v>623</v>
+      </c>
+      <c r="E1" s="154" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="155" t="s">
+        <v>625</v>
+      </c>
+      <c r="B2" s="155" t="s">
+        <v>626</v>
+      </c>
+      <c r="C2" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="155" t="n">
+        <v>18715</v>
+      </c>
+      <c r="E2" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G2" s="153" t="str">
+        <f aca="false">CONCATENATE(A2, " ",B2)</f>
+        <v>ALABA CASTAÑEDA WESLEY</v>
+      </c>
+      <c r="H2" s="155" t="str">
+        <f aca="false">CONCATENATE(G2,"::",C2,"::",D2,"::",E2)</f>
+        <v>ALABA CASTAÑEDA WESLEY::CIRUJANO DENTISTA::18715::xyz</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="155" t="s">
+        <v>627</v>
+      </c>
+      <c r="B3" s="155" t="s">
+        <v>628</v>
+      </c>
+      <c r="C3" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="155" t="n">
+        <v>9108</v>
+      </c>
+      <c r="E3" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G3" s="153" t="str">
+        <f aca="false">CONCATENATE(A3, " ",B3)</f>
+        <v>ALFARO SHIGUETO HOWARD</v>
+      </c>
+      <c r="H3" s="155" t="str">
+        <f aca="false">CONCATENATE(G3,"::",C3,"::",D3,"::",E3)</f>
+        <v>ALFARO SHIGUETO HOWARD::CIRUJANO DENTISTA::9108::xyz</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="155" t="s">
+        <v>629</v>
+      </c>
+      <c r="B4" s="155" t="s">
+        <v>630</v>
+      </c>
+      <c r="C4" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="155" t="n">
+        <v>17832</v>
+      </c>
+      <c r="E4" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G4" s="153" t="str">
+        <f aca="false">CONCATENATE(A4, " ",B4)</f>
+        <v>ANGELES SOTELO MILAGROS ELISA</v>
+      </c>
+      <c r="H4" s="155" t="str">
+        <f aca="false">CONCATENATE(G4,"::",C4,"::",D4,"::",E4)</f>
+        <v>ANGELES SOTELO MILAGROS ELISA::CIRUJANO DENTISTA::17832::xyz</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="155" t="s">
+        <v>631</v>
+      </c>
+      <c r="B5" s="155" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="155" t="n">
+        <v>8233</v>
+      </c>
+      <c r="E5" s="155" t="n">
+        <v>220</v>
+      </c>
+      <c r="G5" s="153" t="str">
+        <f aca="false">CONCATENATE(A5, " ",B5)</f>
+        <v>ARROYO RONCAL FRANCISCO JAVIER</v>
+      </c>
+      <c r="H5" s="155" t="str">
+        <f aca="false">CONCATENATE(G5,"::",C5,"::",D5,"::",E5)</f>
+        <v>ARROYO RONCAL FRANCISCO JAVIER::CIRUJANO DENTISTA::8233::220</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="155" t="s">
+        <v>632</v>
+      </c>
+      <c r="B6" s="155" t="s">
+        <v>360</v>
+      </c>
+      <c r="C6" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="155" t="n">
+        <v>10360</v>
+      </c>
+      <c r="E6" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G6" s="153" t="str">
+        <f aca="false">CONCATENATE(A6, " ",B6)</f>
+        <v>AZULA WONG ERIKA</v>
+      </c>
+      <c r="H6" s="155" t="str">
+        <f aca="false">CONCATENATE(G6,"::",C6,"::",D6,"::",E6)</f>
+        <v>AZULA WONG ERIKA::CIRUJANO DENTISTA::10360::xyz</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="155" t="s">
+        <v>632</v>
+      </c>
+      <c r="B7" s="155" t="s">
+        <v>402</v>
+      </c>
+      <c r="C7" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="155" t="n">
+        <v>13872</v>
+      </c>
+      <c r="E7" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G7" s="153" t="str">
+        <f aca="false">CONCATENATE(A7, " ",B7)</f>
+        <v>AZULA WONG SHIRLEY</v>
+      </c>
+      <c r="H7" s="155" t="str">
+        <f aca="false">CONCATENATE(G7,"::",C7,"::",D7,"::",E7)</f>
+        <v>AZULA WONG SHIRLEY::CIRUJANO DENTISTA::13872::xyz</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="155" t="s">
+        <v>633</v>
+      </c>
+      <c r="B8" s="155" t="s">
+        <v>634</v>
+      </c>
+      <c r="C8" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="155" t="n">
+        <v>5187</v>
+      </c>
+      <c r="E8" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G8" s="153" t="str">
+        <f aca="false">CONCATENATE(A8, " ",B8)</f>
+        <v>CORONEL AMADO MANUEL</v>
+      </c>
+      <c r="H8" s="155" t="str">
+        <f aca="false">CONCATENATE(G8,"::",C8,"::",D8,"::",E8)</f>
+        <v>CORONEL AMADO MANUEL::CIRUJANO DENTISTA::5187::xyz</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="155" t="s">
+        <v>635</v>
+      </c>
+      <c r="B9" s="155" t="s">
+        <v>636</v>
+      </c>
+      <c r="C9" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="155" t="n">
+        <v>11915</v>
+      </c>
+      <c r="E9" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G9" s="153" t="str">
+        <f aca="false">CONCATENATE(A9, " ",B9)</f>
+        <v>CAMPANA MEDINA LUIS</v>
+      </c>
+      <c r="H9" s="155" t="str">
+        <f aca="false">CONCATENATE(G9,"::",C9,"::",D9,"::",E9)</f>
+        <v>CAMPANA MEDINA LUIS::CIRUJANO DENTISTA::11915::xyz</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="155" t="s">
+        <v>637</v>
+      </c>
+      <c r="B10" s="155" t="s">
+        <v>638</v>
+      </c>
+      <c r="C10" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="155" t="n">
+        <v>10262</v>
+      </c>
+      <c r="E10" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G10" s="153" t="str">
+        <f aca="false">CONCATENATE(A10, " ",B10)</f>
+        <v>CRIBILLERO DE PINHO ROSSANA MARLENE</v>
+      </c>
+      <c r="H10" s="155" t="str">
+        <f aca="false">CONCATENATE(G10,"::",C10,"::",D10,"::",E10)</f>
+        <v>CRIBILLERO DE PINHO ROSSANA MARLENE::CIRUJANO DENTISTA::10262::xyz</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="155" t="s">
+        <v>639</v>
+      </c>
+      <c r="B11" s="155" t="s">
+        <v>640</v>
+      </c>
+      <c r="C11" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="155" t="n">
+        <v>5058</v>
+      </c>
+      <c r="E11" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G11" s="153" t="str">
+        <f aca="false">CONCATENATE(A11, " ",B11)</f>
+        <v>DOMINGUEZ ESTRADA MARTIN</v>
+      </c>
+      <c r="H11" s="155" t="str">
+        <f aca="false">CONCATENATE(G11,"::",C11,"::",D11,"::",E11)</f>
+        <v>DOMINGUEZ ESTRADA MARTIN::CIRUJANO DENTISTA::5058::xyz</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="155" t="s">
+        <v>641</v>
+      </c>
+      <c r="B12" s="155" t="s">
+        <v>642</v>
+      </c>
+      <c r="C12" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="155" t="n">
+        <v>14162</v>
+      </c>
+      <c r="E12" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G12" s="153" t="str">
+        <f aca="false">CONCATENATE(A12, " ",B12)</f>
+        <v>FERNANDEZ CASTILLO JULIO IVAN</v>
+      </c>
+      <c r="H12" s="155" t="str">
+        <f aca="false">CONCATENATE(G12,"::",C12,"::",D12,"::",E12)</f>
+        <v>FERNANDEZ CASTILLO JULIO IVAN::CIRUJANO DENTISTA::14162::xyz</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="155" t="s">
+        <v>643</v>
+      </c>
+      <c r="B13" s="155" t="s">
+        <v>644</v>
+      </c>
+      <c r="C13" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="155" t="n">
+        <v>10924</v>
+      </c>
+      <c r="E13" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G13" s="153" t="str">
+        <f aca="false">CONCATENATE(A13, " ",B13)</f>
+        <v>FERNANDEZ TORRES CAROLA</v>
+      </c>
+      <c r="H13" s="155" t="str">
+        <f aca="false">CONCATENATE(G13,"::",C13,"::",D13,"::",E13)</f>
+        <v>FERNANDEZ TORRES CAROLA::CIRUJANO DENTISTA::10924::xyz</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="155" t="s">
+        <v>645</v>
+      </c>
+      <c r="B14" s="155" t="s">
+        <v>646</v>
+      </c>
+      <c r="C14" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="155" t="n">
+        <v>5389</v>
+      </c>
+      <c r="E14" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G14" s="153" t="str">
+        <f aca="false">CONCATENATE(A14, " ",B14)</f>
+        <v>FLORES MENA GABRIEL</v>
+      </c>
+      <c r="H14" s="155" t="str">
+        <f aca="false">CONCATENATE(G14,"::",C14,"::",D14,"::",E14)</f>
+        <v>FLORES MENA GABRIEL::CIRUJANO DENTISTA::5389::xyz</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="155" t="s">
+        <v>647</v>
+      </c>
+      <c r="B15" s="155" t="s">
+        <v>648</v>
+      </c>
+      <c r="C15" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="155" t="n">
+        <v>11325</v>
+      </c>
+      <c r="E15" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G15" s="153" t="str">
+        <f aca="false">CONCATENATE(A15, " ",B15)</f>
+        <v>GYGLI REINA WALTER</v>
+      </c>
+      <c r="H15" s="155" t="str">
+        <f aca="false">CONCATENATE(G15,"::",C15,"::",D15,"::",E15)</f>
+        <v>GYGLI REINA WALTER::CIRUJANO DENTISTA::11325::xyz</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="155" t="s">
+        <v>649</v>
+      </c>
+      <c r="B16" s="155" t="s">
+        <v>650</v>
+      </c>
+      <c r="C16" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="155" t="n">
+        <v>19510</v>
+      </c>
+      <c r="E16" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G16" s="153" t="str">
+        <f aca="false">CONCATENATE(A16, " ",B16)</f>
+        <v>LANFRANCO LEON ALFREDO</v>
+      </c>
+      <c r="H16" s="155" t="str">
+        <f aca="false">CONCATENATE(G16,"::",C16,"::",D16,"::",E16)</f>
+        <v>LANFRANCO LEON ALFREDO::CIRUJANO DENTISTA::19510::xyz</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="155" t="s">
+        <v>651</v>
+      </c>
+      <c r="B17" s="155" t="s">
+        <v>652</v>
+      </c>
+      <c r="C17" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="155" t="n">
+        <v>15877</v>
+      </c>
+      <c r="E17" s="155" t="n">
+        <v>2232</v>
+      </c>
+      <c r="G17" s="153" t="str">
+        <f aca="false">CONCATENATE(A17, " ",B17)</f>
+        <v>LLERENA PEREZ LOURDES</v>
+      </c>
+      <c r="H17" s="155" t="str">
+        <f aca="false">CONCATENATE(G17,"::",C17,"::",D17,"::",E17)</f>
+        <v>LLERENA PEREZ LOURDES::CIRUJANO DENTISTA::15877::2232</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="155" t="s">
+        <v>653</v>
+      </c>
+      <c r="B18" s="155" t="s">
+        <v>654</v>
+      </c>
+      <c r="C18" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="155" t="n">
+        <v>19300</v>
+      </c>
+      <c r="E18" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G18" s="153" t="str">
+        <f aca="false">CONCATENATE(A18, " ",B18)</f>
+        <v>MANRIQUE CHAVEZ CAROLINA</v>
+      </c>
+      <c r="H18" s="155" t="str">
+        <f aca="false">CONCATENATE(G18,"::",C18,"::",D18,"::",E18)</f>
+        <v>MANRIQUE CHAVEZ CAROLINA::CIRUJANO DENTISTA::19300::xyz</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="155" t="s">
+        <v>655</v>
+      </c>
+      <c r="B19" s="155" t="s">
+        <v>656</v>
+      </c>
+      <c r="C19" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="155" t="n">
+        <v>10819</v>
+      </c>
+      <c r="E19" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G19" s="153" t="str">
+        <f aca="false">CONCATENATE(A19, " ",B19)</f>
+        <v>MARQUEZ MENDOZA ALEXIS</v>
+      </c>
+      <c r="H19" s="155" t="str">
+        <f aca="false">CONCATENATE(G19,"::",C19,"::",D19,"::",E19)</f>
+        <v>MARQUEZ MENDOZA ALEXIS::CIRUJANO DENTISTA::10819::xyz</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="155" t="s">
+        <v>657</v>
+      </c>
+      <c r="B20" s="155" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="155" t="n">
+        <v>16797</v>
+      </c>
+      <c r="E20" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G20" s="153" t="str">
+        <f aca="false">CONCATENATE(A20, " ",B20)</f>
+        <v>ORTIZ PALOMINO LUIS ALEJANDRO</v>
+      </c>
+      <c r="H20" s="155" t="str">
+        <f aca="false">CONCATENATE(G20,"::",C20,"::",D20,"::",E20)</f>
+        <v>ORTIZ PALOMINO LUIS ALEJANDRO::CIRUJANO DENTISTA::16797::xyz</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="155" t="s">
+        <v>658</v>
+      </c>
+      <c r="B21" s="155" t="s">
+        <v>659</v>
+      </c>
+      <c r="C21" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="155" t="n">
+        <v>20232</v>
+      </c>
+      <c r="E21" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G21" s="153" t="str">
+        <f aca="false">CONCATENATE(A21, " ",B21)</f>
+        <v>OLIVERA MADGE LUIS ENRIQUE</v>
+      </c>
+      <c r="H21" s="155" t="str">
+        <f aca="false">CONCATENATE(G21,"::",C21,"::",D21,"::",E21)</f>
+        <v>OLIVERA MADGE LUIS ENRIQUE::CIRUJANO DENTISTA::20232::xyz</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="155" t="s">
+        <v>660</v>
+      </c>
+      <c r="B22" s="155" t="s">
+        <v>636</v>
+      </c>
+      <c r="C22" s="155" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="155" t="n">
+        <v>8250</v>
+      </c>
+      <c r="E22" s="155" t="n">
+        <v>463</v>
+      </c>
+      <c r="G22" s="153" t="str">
+        <f aca="false">CONCATENATE(A22, " ",B22)</f>
+        <v>PIAGGIO BRAVO LUIS</v>
+      </c>
+      <c r="H22" s="155" t="str">
+        <f aca="false">CONCATENATE(G22,"::",C22,"::",D22,"::",E22)</f>
+        <v>PIAGGIO BRAVO LUIS::IMPLANTOLOGIA ORAL INTEGRAL::8250::463</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="155" t="s">
+        <v>661</v>
+      </c>
+      <c r="B23" s="155" t="s">
+        <v>636</v>
+      </c>
+      <c r="C23" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="155" t="n">
+        <v>15456</v>
+      </c>
+      <c r="E23" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G23" s="153" t="str">
+        <f aca="false">CONCATENATE(A23, " ",B23)</f>
+        <v>RAGGIO BENAVIDES LUIS</v>
+      </c>
+      <c r="H23" s="155" t="str">
+        <f aca="false">CONCATENATE(G23,"::",C23,"::",D23,"::",E23)</f>
+        <v>RAGGIO BENAVIDES LUIS::CIRUJANO DENTISTA::15456::xyz</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="155" t="s">
+        <v>662</v>
+      </c>
+      <c r="B24" s="155" t="s">
+        <v>663</v>
+      </c>
+      <c r="C24" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="155" t="n">
+        <v>1693</v>
+      </c>
+      <c r="E24" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G24" s="153" t="str">
+        <f aca="false">CONCATENATE(A24, " ",B24)</f>
+        <v>SALAZAR GARCIA JAVIER FRANCISCO</v>
+      </c>
+      <c r="H24" s="155" t="str">
+        <f aca="false">CONCATENATE(G24,"::",C24,"::",D24,"::",E24)</f>
+        <v>SALAZAR GARCIA JAVIER FRANCISCO::CIRUJANO DENTISTA::1693::xyz</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="155" t="s">
+        <v>664</v>
+      </c>
+      <c r="B25" s="155" t="s">
+        <v>665</v>
+      </c>
+      <c r="C25" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="155" t="n">
+        <v>24119</v>
+      </c>
+      <c r="E25" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G25" s="153" t="str">
+        <f aca="false">CONCATENATE(A25, " ",B25)</f>
+        <v>SCARAFONE ALVIS GERSON GIANCARLO</v>
+      </c>
+      <c r="H25" s="155" t="str">
+        <f aca="false">CONCATENATE(G25,"::",C25,"::",D25,"::",E25)</f>
+        <v>SCARAFONE ALVIS GERSON GIANCARLO::CIRUJANO DENTISTA::24119::xyz</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="155" t="s">
+        <v>666</v>
+      </c>
+      <c r="B26" s="155" t="s">
+        <v>636</v>
+      </c>
+      <c r="C26" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="155" t="n">
+        <v>13240</v>
+      </c>
+      <c r="E26" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G26" s="153" t="str">
+        <f aca="false">CONCATENATE(A26, " ",B26)</f>
+        <v>TAFUR JIMENEZ LUIS</v>
+      </c>
+      <c r="H26" s="155" t="str">
+        <f aca="false">CONCATENATE(G26,"::",C26,"::",D26,"::",E26)</f>
+        <v>TAFUR JIMENEZ LUIS::CIRUJANO DENTISTA::13240::xyz</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="155" t="s">
+        <v>667</v>
+      </c>
+      <c r="B27" s="155" t="s">
+        <v>563</v>
+      </c>
+      <c r="C27" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="155" t="n">
+        <v>5177</v>
+      </c>
+      <c r="E27" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G27" s="153" t="str">
+        <f aca="false">CONCATENATE(A27, " ",B27)</f>
+        <v>VIVES BARRETO VICTOR HUGO</v>
+      </c>
+      <c r="H27" s="155" t="str">
+        <f aca="false">CONCATENATE(G27,"::",C27,"::",D27,"::",E27)</f>
+        <v>VIVES BARRETO VICTOR HUGO::CIRUJANO DENTISTA::5177::xyz</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="155" t="s">
+        <v>668</v>
+      </c>
+      <c r="B28" s="155" t="s">
+        <v>650</v>
+      </c>
+      <c r="C28" s="155" t="s">
+        <v>669</v>
+      </c>
+      <c r="D28" s="155" t="n">
+        <v>15895</v>
+      </c>
+      <c r="E28" s="155" t="n">
+        <v>402</v>
+      </c>
+      <c r="G28" s="153" t="str">
+        <f aca="false">CONCATENATE(A28, " ",B28)</f>
+        <v>ZUIKO FELIX ALFREDO</v>
+      </c>
+      <c r="H28" s="155" t="str">
+        <f aca="false">CONCATENATE(G28,"::",C28,"::",D28,"::",E28)</f>
+        <v>ZUIKO FELIX ALFREDO::CIRUGÍA BUCAL Y MAXILO FACIAL::15895::402</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="155" t="s">
+        <v>670</v>
+      </c>
+      <c r="B29" s="155" t="s">
+        <v>303</v>
+      </c>
+      <c r="C29" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="155" t="n">
+        <v>13806</v>
+      </c>
+      <c r="E29" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G29" s="153" t="str">
+        <f aca="false">CONCATENATE(A29, " ",B29)</f>
+        <v>PIÑA CARDENAS JORGE LUIS</v>
+      </c>
+      <c r="H29" s="155" t="str">
+        <f aca="false">CONCATENATE(G29,"::",C29,"::",D29,"::",E29)</f>
+        <v>PIÑA CARDENAS JORGE LUIS::CIRUJANO DENTISTA::13806::xyz</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="155" t="s">
+        <v>671</v>
+      </c>
+      <c r="B30" s="155" t="s">
+        <v>672</v>
+      </c>
+      <c r="C30" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="155" t="n">
+        <v>28049</v>
+      </c>
+      <c r="E30" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G30" s="153" t="str">
+        <f aca="false">CONCATENATE(A30, " ",B30)</f>
+        <v>ALMEIDA RUIZ CLAUDIA</v>
+      </c>
+      <c r="H30" s="155" t="str">
+        <f aca="false">CONCATENATE(G30,"::",C30,"::",D30,"::",E30)</f>
+        <v>ALMEIDA RUIZ CLAUDIA::CIRUJANO DENTISTA::28049::xyz</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="155" t="s">
+        <v>673</v>
+      </c>
+      <c r="B31" s="155" t="s">
+        <v>674</v>
+      </c>
+      <c r="C31" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="155" t="n">
+        <v>28240</v>
+      </c>
+      <c r="E31" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G31" s="153" t="str">
+        <f aca="false">CONCATENATE(A31, " ",B31)</f>
+        <v>AYRES TORANZO ANDREA</v>
+      </c>
+      <c r="H31" s="155" t="str">
+        <f aca="false">CONCATENATE(G31,"::",C31,"::",D31,"::",E31)</f>
+        <v>AYRES TORANZO ANDREA::CIRUJANO DENTISTA::28240::xyz</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="155" t="s">
+        <v>675</v>
+      </c>
+      <c r="B32" s="155" t="s">
+        <v>676</v>
+      </c>
+      <c r="C32" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="155" t="n">
+        <v>7224</v>
+      </c>
+      <c r="E32" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G32" s="153" t="str">
+        <f aca="false">CONCATENATE(A32, " ",B32)</f>
+        <v>MARCHANI MARQUEZ MILUZKA</v>
+      </c>
+      <c r="H32" s="155" t="str">
+        <f aca="false">CONCATENATE(G32,"::",C32,"::",D32,"::",E32)</f>
+        <v>MARCHANI MARQUEZ MILUZKA::CIRUJANO DENTISTA::7224::xyz</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="155" t="s">
+        <v>677</v>
+      </c>
+      <c r="B33" s="155" t="s">
+        <v>678</v>
+      </c>
+      <c r="C33" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="155" t="n">
+        <v>4553</v>
+      </c>
+      <c r="E33" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G33" s="153" t="str">
+        <f aca="false">CONCATENATE(A33, " ",B33)</f>
+        <v>ROJAS AMADO MARITZA</v>
+      </c>
+      <c r="H33" s="155" t="str">
+        <f aca="false">CONCATENATE(G33,"::",C33,"::",D33,"::",E33)</f>
+        <v>ROJAS AMADO MARITZA::CIRUJANO DENTISTA::4553::xyz</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="155" t="s">
+        <v>679</v>
+      </c>
+      <c r="B34" s="155" t="s">
+        <v>680</v>
+      </c>
+      <c r="C34" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="155" t="n">
+        <v>26850</v>
+      </c>
+      <c r="E34" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G34" s="153" t="str">
+        <f aca="false">CONCATENATE(A34, " ",B34)</f>
+        <v>SANTOS SALAS ELENA</v>
+      </c>
+      <c r="H34" s="155" t="str">
+        <f aca="false">CONCATENATE(G34,"::",C34,"::",D34,"::",E34)</f>
+        <v>SANTOS SALAS ELENA::CIRUJANO DENTISTA::26850::xyz</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="155" t="s">
+        <v>681</v>
+      </c>
+      <c r="B35" s="155" t="s">
+        <v>682</v>
+      </c>
+      <c r="C35" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="155" t="n">
+        <v>6280</v>
+      </c>
+      <c r="E35" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G35" s="153" t="str">
+        <f aca="false">CONCATENATE(A35, " ",B35)</f>
+        <v>SANTOS ESCALANTE CLAVER</v>
+      </c>
+      <c r="H35" s="155" t="str">
+        <f aca="false">CONCATENATE(G35,"::",C35,"::",D35,"::",E35)</f>
+        <v>SANTOS ESCALANTE CLAVER::CIRUJANO DENTISTA::6280::xyz</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="155" t="s">
+        <v>683</v>
+      </c>
+      <c r="B36" s="155" t="s">
+        <v>684</v>
+      </c>
+      <c r="C36" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="155" t="n">
+        <v>43088</v>
+      </c>
+      <c r="E36" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G36" s="153" t="str">
+        <f aca="false">CONCATENATE(A36, " ",B36)</f>
+        <v>ARCE SILVA HUBERTO GONZALO</v>
+      </c>
+      <c r="H36" s="155" t="str">
+        <f aca="false">CONCATENATE(G36,"::",C36,"::",D36,"::",E36)</f>
+        <v>ARCE SILVA HUBERTO GONZALO::CIRUJANO DENTISTA::43088::xyz</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="155" t="s">
+        <v>685</v>
+      </c>
+      <c r="B37" s="155" t="s">
+        <v>686</v>
+      </c>
+      <c r="C37" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="155" t="n">
+        <v>28153</v>
+      </c>
+      <c r="E37" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G37" s="153" t="str">
+        <f aca="false">CONCATENATE(A37, " ",B37)</f>
+        <v>PAUCCA MONTOYA CINTHYA</v>
+      </c>
+      <c r="H37" s="155" t="str">
+        <f aca="false">CONCATENATE(G37,"::",C37,"::",D37,"::",E37)</f>
+        <v>PAUCCA MONTOYA CINTHYA::CIRUJANO DENTISTA::28153::xyz</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="155" t="s">
+        <v>687</v>
+      </c>
+      <c r="B38" s="155" t="s">
+        <v>688</v>
+      </c>
+      <c r="C38" s="155" t="s">
+        <v>669</v>
+      </c>
+      <c r="D38" s="155" t="n">
+        <v>23825</v>
+      </c>
+      <c r="E38" s="155" t="n">
+        <v>1380</v>
+      </c>
+      <c r="G38" s="153" t="str">
+        <f aca="false">CONCATENATE(A38, " ",B38)</f>
+        <v>VADILLO PALACIOS GRISEL YULIANA</v>
+      </c>
+      <c r="H38" s="155" t="str">
+        <f aca="false">CONCATENATE(G38,"::",C38,"::",D38,"::",E38)</f>
+        <v>VADILLO PALACIOS GRISEL YULIANA::CIRUGÍA BUCAL Y MAXILO FACIAL::23825::1380</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="155" t="s">
+        <v>689</v>
+      </c>
+      <c r="B39" s="155" t="s">
+        <v>690</v>
+      </c>
+      <c r="C39" s="155" t="s">
+        <v>691</v>
+      </c>
+      <c r="D39" s="155" t="n">
+        <v>22288</v>
+      </c>
+      <c r="E39" s="155" t="n">
+        <v>1559</v>
+      </c>
+      <c r="G39" s="153" t="str">
+        <f aca="false">CONCATENATE(A39, " ",B39)</f>
+        <v>VELEZMORO PEÑA ELVIRA VANESSA</v>
+      </c>
+      <c r="H39" s="155" t="str">
+        <f aca="false">CONCATENATE(G39,"::",C39,"::",D39,"::",E39)</f>
+        <v>VELEZMORO PEÑA ELVIRA VANESSA::ODONTOPEDIATRÍA::22288::1559</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="155" t="s">
+        <v>692</v>
+      </c>
+      <c r="B40" s="155" t="s">
+        <v>693</v>
+      </c>
+      <c r="C40" s="155" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="155" t="n">
+        <v>10064</v>
+      </c>
+      <c r="E40" s="155" t="n">
+        <v>78</v>
+      </c>
+      <c r="G40" s="153" t="str">
+        <f aca="false">CONCATENATE(A40, " ",B40)</f>
+        <v>TAFUR TAFUR ALY MICHEL</v>
+      </c>
+      <c r="H40" s="155" t="str">
+        <f aca="false">CONCATENATE(G40,"::",C40,"::",D40,"::",E40)</f>
+        <v>TAFUR TAFUR ALY MICHEL::ORTODONCIA::10064::78</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="155" t="s">
+        <v>694</v>
+      </c>
+      <c r="B41" s="155" t="s">
+        <v>280</v>
+      </c>
+      <c r="C41" s="155" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="155" t="n">
+        <v>18550</v>
+      </c>
+      <c r="E41" s="155" t="n">
+        <v>763</v>
+      </c>
+      <c r="G41" s="153" t="str">
+        <f aca="false">CONCATENATE(A41, " ",B41)</f>
+        <v>SILVA ALBIZURI CESAR CHRISTIAN</v>
+      </c>
+      <c r="H41" s="155" t="str">
+        <f aca="false">CONCATENATE(G41,"::",C41,"::",D41,"::",E41)</f>
+        <v>SILVA ALBIZURI CESAR CHRISTIAN::ORTODONCIA::18550::763</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="155" t="s">
+        <v>679</v>
+      </c>
+      <c r="B42" s="155" t="s">
+        <v>326</v>
+      </c>
+      <c r="C42" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="155" t="n">
+        <v>31076</v>
+      </c>
+      <c r="E42" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G42" s="153" t="str">
+        <f aca="false">CONCATENATE(A42, " ",B42)</f>
+        <v>SANTOS SALAS CECILIA PIA</v>
+      </c>
+      <c r="H42" s="155" t="str">
+        <f aca="false">CONCATENATE(G42,"::",C42,"::",D42,"::",E42)</f>
+        <v>SANTOS SALAS CECILIA PIA::CIRUJANO DENTISTA::31076::xyz</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="155" t="s">
+        <v>695</v>
+      </c>
+      <c r="B43" s="155" t="s">
+        <v>696</v>
+      </c>
+      <c r="C43" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="155" t="n">
+        <v>17703</v>
+      </c>
+      <c r="E43" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G43" s="153" t="str">
+        <f aca="false">CONCATENATE(A43, " ",B43)</f>
+        <v>RIVERA ALIAGA ALVARO</v>
+      </c>
+      <c r="H43" s="155" t="str">
+        <f aca="false">CONCATENATE(G43,"::",C43,"::",D43,"::",E43)</f>
+        <v>RIVERA ALIAGA ALVARO::CIRUJANO DENTISTA::17703::xyz</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="155" t="s">
+        <v>697</v>
+      </c>
+      <c r="B44" s="155" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="155" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="155" t="n">
+        <v>11811</v>
+      </c>
+      <c r="E44" s="155" t="n">
+        <v>79</v>
+      </c>
+      <c r="G44" s="153" t="str">
+        <f aca="false">CONCATENATE(A44, " ",B44)</f>
+        <v>RAYMUNDO CALERO JULIO</v>
+      </c>
+      <c r="H44" s="155" t="str">
+        <f aca="false">CONCATENATE(G44,"::",C44,"::",D44,"::",E44)</f>
+        <v>RAYMUNDO CALERO JULIO::ORTODONCIA::11811::79</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="155" t="s">
+        <v>698</v>
+      </c>
+      <c r="B45" s="155" t="s">
+        <v>699</v>
+      </c>
+      <c r="C45" s="155" t="s">
+        <v>700</v>
+      </c>
+      <c r="D45" s="155" t="n">
+        <v>21650</v>
+      </c>
+      <c r="E45" s="155" t="n">
+        <v>2602</v>
+      </c>
+      <c r="G45" s="153" t="str">
+        <f aca="false">CONCATENATE(A45, " ",B45)</f>
+        <v>RAMIREZ MASIAS NATHALY MILAGROS</v>
+      </c>
+      <c r="H45" s="155" t="str">
+        <f aca="false">CONCATENATE(G45,"::",C45,"::",D45,"::",E45)</f>
+        <v>RAMIREZ MASIAS NATHALY MILAGROS::REHABILITACIÓN ORAL::21650::2602</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="155" t="s">
+        <v>701</v>
+      </c>
+      <c r="B46" s="155" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="155" t="n">
+        <v>6218</v>
+      </c>
+      <c r="E46" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G46" s="153" t="str">
+        <f aca="false">CONCATENATE(A46, " ",B46)</f>
+        <v>PAZ MAYURI CARLOS ALBERTO</v>
+      </c>
+      <c r="H46" s="155" t="str">
+        <f aca="false">CONCATENATE(G46,"::",C46,"::",D46,"::",E46)</f>
+        <v>PAZ MAYURI CARLOS ALBERTO::CIRUJANO DENTISTA::6218::xyz</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="155" t="s">
+        <v>702</v>
+      </c>
+      <c r="B47" s="155" t="s">
+        <v>703</v>
+      </c>
+      <c r="C47" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="155" t="n">
+        <v>30542</v>
+      </c>
+      <c r="E47" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G47" s="153" t="str">
+        <f aca="false">CONCATENATE(A47, " ",B47)</f>
+        <v>PAJARES MUÑOZ CLAUDIA MAGALI</v>
+      </c>
+      <c r="H47" s="155" t="str">
+        <f aca="false">CONCATENATE(G47,"::",C47,"::",D47,"::",E47)</f>
+        <v>PAJARES MUÑOZ CLAUDIA MAGALI::CIRUJANO DENTISTA::30542::xyz</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="155" t="s">
+        <v>704</v>
+      </c>
+      <c r="B48" s="155" t="s">
+        <v>672</v>
+      </c>
+      <c r="C48" s="155" t="s">
+        <v>691</v>
+      </c>
+      <c r="D48" s="155" t="n">
+        <v>14519</v>
+      </c>
+      <c r="E48" s="155" t="n">
+        <v>626</v>
+      </c>
+      <c r="G48" s="153" t="str">
+        <f aca="false">CONCATENATE(A48, " ",B48)</f>
+        <v>OTAZU ALDANA CLAUDIA</v>
+      </c>
+      <c r="H48" s="155" t="str">
+        <f aca="false">CONCATENATE(G48,"::",C48,"::",D48,"::",E48)</f>
+        <v>OTAZU ALDANA CLAUDIA::ODONTOPEDIATRÍA::14519::626</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="155" t="s">
+        <v>705</v>
+      </c>
+      <c r="B49" s="155" t="s">
+        <v>706</v>
+      </c>
+      <c r="C49" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="155" t="n">
+        <v>9072</v>
+      </c>
+      <c r="E49" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G49" s="153" t="str">
+        <f aca="false">CONCATENATE(A49, " ",B49)</f>
+        <v>MOSCOL GALLARDO FERNANDO JAVIER</v>
+      </c>
+      <c r="H49" s="155" t="str">
+        <f aca="false">CONCATENATE(G49,"::",C49,"::",D49,"::",E49)</f>
+        <v>MOSCOL GALLARDO FERNANDO JAVIER::CIRUJANO DENTISTA::9072::xyz</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="155" t="s">
+        <v>707</v>
+      </c>
+      <c r="B50" s="155" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="155" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="155" t="n">
+        <v>573</v>
+      </c>
+      <c r="E50" s="155" t="n">
+        <v>14</v>
+      </c>
+      <c r="G50" s="153" t="str">
+        <f aca="false">CONCATENATE(A50, " ",B50)</f>
+        <v>MENESES LOPEZ ABRAHAM</v>
+      </c>
+      <c r="H50" s="155" t="str">
+        <f aca="false">CONCATENATE(G50,"::",C50,"::",D50,"::",E50)</f>
+        <v>MENESES LOPEZ ABRAHAM::ORTODONCIA::573::14</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="155" t="s">
+        <v>708</v>
+      </c>
+      <c r="B51" s="155" t="s">
+        <v>709</v>
+      </c>
+      <c r="C51" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="155" t="n">
+        <v>12799</v>
+      </c>
+      <c r="E51" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G51" s="153" t="str">
+        <f aca="false">CONCATENATE(A51, " ",B51)</f>
+        <v>GUILLEN ASTETE CELSO ANTONIO</v>
+      </c>
+      <c r="H51" s="155" t="str">
+        <f aca="false">CONCATENATE(G51,"::",C51,"::",D51,"::",E51)</f>
+        <v>GUILLEN ASTETE CELSO ANTONIO::CIRUJANO DENTISTA::12799::xyz</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="155" t="s">
+        <v>710</v>
+      </c>
+      <c r="B52" s="155" t="s">
+        <v>711</v>
+      </c>
+      <c r="C52" s="155" t="s">
+        <v>691</v>
+      </c>
+      <c r="D52" s="155" t="n">
+        <v>25379</v>
+      </c>
+      <c r="E52" s="155" t="n">
+        <v>1824</v>
+      </c>
+      <c r="G52" s="153" t="str">
+        <f aca="false">CONCATENATE(A52, " ",B52)</f>
+        <v>GALVEZ CUBAS GISELA ELIZABETH</v>
+      </c>
+      <c r="H52" s="155" t="str">
+        <f aca="false">CONCATENATE(G52,"::",C52,"::",D52,"::",E52)</f>
+        <v>GALVEZ CUBAS GISELA ELIZABETH::ODONTOPEDIATRÍA::25379::1824</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="155" t="s">
+        <v>712</v>
+      </c>
+      <c r="B53" s="155" t="s">
+        <v>713</v>
+      </c>
+      <c r="C53" s="155" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="155" t="n">
+        <v>26784</v>
+      </c>
+      <c r="E53" s="155" t="n">
+        <v>2188</v>
+      </c>
+      <c r="G53" s="153" t="str">
+        <f aca="false">CONCATENATE(A53, " ",B53)</f>
+        <v>FLORES RICARDI GABRIEL PEDRO</v>
+      </c>
+      <c r="H53" s="155" t="str">
+        <f aca="false">CONCATENATE(G53,"::",C53,"::",D53,"::",E53)</f>
+        <v>FLORES RICARDI GABRIEL PEDRO::ORTODONCIA::26784::2188</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="155" t="s">
+        <v>714</v>
+      </c>
+      <c r="B54" s="155" t="s">
+        <v>715</v>
+      </c>
+      <c r="C54" s="155" t="s">
+        <v>691</v>
+      </c>
+      <c r="D54" s="155" t="n">
+        <v>6833</v>
+      </c>
+      <c r="E54" s="155" t="n">
+        <v>10</v>
+      </c>
+      <c r="G54" s="153" t="str">
+        <f aca="false">CONCATENATE(A54, " ",B54)</f>
+        <v>FLORES MORENO MARTHA</v>
+      </c>
+      <c r="H54" s="155" t="str">
+        <f aca="false">CONCATENATE(G54,"::",C54,"::",D54,"::",E54)</f>
+        <v>FLORES MORENO MARTHA::ODONTOPEDIATRÍA::6833::10</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="155" t="s">
+        <v>716</v>
+      </c>
+      <c r="B55" s="155" t="s">
+        <v>717</v>
+      </c>
+      <c r="C55" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="155" t="n">
+        <v>6834</v>
+      </c>
+      <c r="E55" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G55" s="153" t="str">
+        <f aca="false">CONCATENATE(A55, " ",B55)</f>
+        <v>CARDENAS MARINO ESTHER</v>
+      </c>
+      <c r="H55" s="155" t="str">
+        <f aca="false">CONCATENATE(G55,"::",C55,"::",D55,"::",E55)</f>
+        <v>CARDENAS MARINO ESTHER::CIRUJANO DENTISTA::6834::xyz</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="155" t="s">
+        <v>718</v>
+      </c>
+      <c r="B56" s="155" t="s">
+        <v>719</v>
+      </c>
+      <c r="C56" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="155" t="n">
+        <v>33621</v>
+      </c>
+      <c r="E56" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G56" s="153" t="str">
+        <f aca="false">CONCATENATE(A56, " ",B56)</f>
+        <v>CALDERON VALENCIA MARIELA ZUNILDA</v>
+      </c>
+      <c r="H56" s="155" t="str">
+        <f aca="false">CONCATENATE(G56,"::",C56,"::",D56,"::",E56)</f>
+        <v>CALDERON VALENCIA MARIELA ZUNILDA::CIRUJANO DENTISTA::33621::xyz</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="155" t="s">
+        <v>718</v>
+      </c>
+      <c r="B57" s="155" t="s">
+        <v>719</v>
+      </c>
+      <c r="C57" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="155" t="n">
+        <v>33621</v>
+      </c>
+      <c r="E57" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G57" s="153" t="str">
+        <f aca="false">CONCATENATE(A57, " ",B57)</f>
+        <v>CALDERON VALENCIA MARIELA ZUNILDA</v>
+      </c>
+      <c r="H57" s="155" t="str">
+        <f aca="false">CONCATENATE(G57,"::",C57,"::",D57,"::",E57)</f>
+        <v>CALDERON VALENCIA MARIELA ZUNILDA::CIRUJANO DENTISTA::33621::xyz</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="155" t="s">
+        <v>718</v>
+      </c>
+      <c r="B58" s="155" t="s">
+        <v>719</v>
+      </c>
+      <c r="C58" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="155" t="n">
+        <v>33621</v>
+      </c>
+      <c r="E58" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G58" s="153" t="str">
+        <f aca="false">CONCATENATE(A58, " ",B58)</f>
+        <v>CALDERON VALENCIA MARIELA ZUNILDA</v>
+      </c>
+      <c r="H58" s="155" t="str">
+        <f aca="false">CONCATENATE(G58,"::",C58,"::",D58,"::",E58)</f>
+        <v>CALDERON VALENCIA MARIELA ZUNILDA::CIRUJANO DENTISTA::33621::xyz</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="155" t="s">
+        <v>718</v>
+      </c>
+      <c r="B59" s="155" t="s">
+        <v>719</v>
+      </c>
+      <c r="C59" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="155" t="n">
+        <v>33621</v>
+      </c>
+      <c r="E59" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G59" s="153" t="str">
+        <f aca="false">CONCATENATE(A59, " ",B59)</f>
+        <v>CALDERON VALENCIA MARIELA ZUNILDA</v>
+      </c>
+      <c r="H59" s="155" t="str">
+        <f aca="false">CONCATENATE(G59,"::",C59,"::",D59,"::",E59)</f>
+        <v>CALDERON VALENCIA MARIELA ZUNILDA::CIRUJANO DENTISTA::33621::xyz</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="155" t="s">
+        <v>720</v>
+      </c>
+      <c r="B60" s="155" t="s">
+        <v>721</v>
+      </c>
+      <c r="C60" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="155" t="n">
+        <v>12732</v>
+      </c>
+      <c r="E60" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G60" s="153" t="str">
+        <f aca="false">CONCATENATE(A60, " ",B60)</f>
+        <v>BAMONDE SEGURA LEYLA</v>
+      </c>
+      <c r="H60" s="155" t="str">
+        <f aca="false">CONCATENATE(G60,"::",C60,"::",D60,"::",E60)</f>
+        <v>BAMONDE SEGURA LEYLA::CIRUJANO DENTISTA::12732::xyz</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="155" t="s">
+        <v>722</v>
+      </c>
+      <c r="B61" s="155" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="155" t="s">
+        <v>114</v>
+      </c>
+      <c r="D61" s="155" t="n">
+        <v>16945</v>
+      </c>
+      <c r="E61" s="155" t="n">
+        <v>855</v>
+      </c>
+      <c r="G61" s="153" t="str">
+        <f aca="false">CONCATENATE(A61, " ",B61)</f>
+        <v>ARRIOLA GUILLEN LUIS ERNESTO</v>
+      </c>
+      <c r="H61" s="155" t="str">
+        <f aca="false">CONCATENATE(G61,"::",C61,"::",D61,"::",E61)</f>
+        <v>ARRIOLA GUILLEN LUIS ERNESTO::ORTODONCIA::16945::855</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="155" t="s">
+        <v>722</v>
+      </c>
+      <c r="B62" s="155" t="s">
+        <v>154</v>
+      </c>
+      <c r="C62" s="155" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" s="155" t="n">
+        <v>16945</v>
+      </c>
+      <c r="E62" s="155" t="n">
+        <v>855</v>
+      </c>
+      <c r="G62" s="153" t="str">
+        <f aca="false">CONCATENATE(A62, " ",B62)</f>
+        <v>ARRIOLA GUILLEN LUIS ERNESTO</v>
+      </c>
+      <c r="H62" s="155" t="str">
+        <f aca="false">CONCATENATE(G62,"::",C62,"::",D62,"::",E62)</f>
+        <v>ARRIOLA GUILLEN LUIS ERNESTO::ORTODONCIA::16945::855</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="155" t="s">
+        <v>722</v>
+      </c>
+      <c r="B63" s="155" t="s">
+        <v>154</v>
+      </c>
+      <c r="C63" s="155" t="s">
+        <v>114</v>
+      </c>
+      <c r="D63" s="155" t="n">
+        <v>16945</v>
+      </c>
+      <c r="E63" s="155" t="n">
+        <v>855</v>
+      </c>
+      <c r="G63" s="153" t="str">
+        <f aca="false">CONCATENATE(A63, " ",B63)</f>
+        <v>ARRIOLA GUILLEN LUIS ERNESTO</v>
+      </c>
+      <c r="H63" s="155" t="str">
+        <f aca="false">CONCATENATE(G63,"::",C63,"::",D63,"::",E63)</f>
+        <v>ARRIOLA GUILLEN LUIS ERNESTO::ORTODONCIA::16945::855</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="155" t="s">
+        <v>723</v>
+      </c>
+      <c r="B64" s="155" t="s">
+        <v>724</v>
+      </c>
+      <c r="C64" s="155" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="155" t="n">
+        <v>45592</v>
+      </c>
+      <c r="E64" s="156" t="s">
+        <v>599</v>
+      </c>
+      <c r="G64" s="153" t="str">
+        <f aca="false">CONCATENATE(A64, " ",B64)</f>
+        <v>ARMAS GALVEZ NELSON MURICIO</v>
+      </c>
+      <c r="H64" s="155" t="str">
+        <f aca="false">CONCATENATE(G64,"::",C64,"::",D64,"::",E64)</f>
+        <v>ARMAS GALVEZ NELSON MURICIO::CIRUJANO DENTISTA::45592::xyz</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="155" t="s">
+        <v>725</v>
+      </c>
+      <c r="B65" s="155" t="s">
+        <v>726</v>
+      </c>
+      <c r="C65" s="155" t="s">
+        <v>691</v>
+      </c>
+      <c r="D65" s="155" t="n">
+        <v>14480</v>
+      </c>
+      <c r="E65" s="155" t="n">
+        <v>455</v>
+      </c>
+      <c r="G65" s="153" t="str">
+        <f aca="false">CONCATENATE(A65, " ",B65)</f>
+        <v>AMARO RIVERA MARIA YESENIA</v>
+      </c>
+      <c r="H65" s="155" t="str">
+        <f aca="false">CONCATENATE(G65,"::",C65,"::",D65,"::",E65)</f>
+        <v>AMARO RIVERA MARIA YESENIA::ODONTOPEDIATRÍA::14480::455</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="155" t="s">
+        <v>727</v>
+      </c>
+      <c r="B66" s="155" t="s">
+        <v>728</v>
+      </c>
+      <c r="C66" s="155" t="s">
+        <v>691</v>
+      </c>
+      <c r="D66" s="155" t="n">
+        <v>24563</v>
+      </c>
+      <c r="E66" s="155" t="n">
+        <v>1627</v>
+      </c>
+      <c r="G66" s="153" t="str">
+        <f aca="false">CONCATENATE(A66, " ",B66)</f>
+        <v>ALVITEZ CABALLERO PAMELA</v>
+      </c>
+      <c r="H66" s="155" t="str">
+        <f aca="false">CONCATENATE(G66,"::",C66,"::",D66,"::",E66)</f>
+        <v>ALVITEZ CABALLERO PAMELA::ODONTOPEDIATRÍA::24563::1627</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>